<commit_message>
tweak paths in test file to work on Rushmore
</commit_message>
<xml_diff>
--- a/tests/input_csv_file_test_case_Evan_simple.xlsx
+++ b/tests/input_csv_file_test_case_Evan_simple.xlsx
@@ -49,19 +49,19 @@
     <t>.</t>
   </si>
   <si>
-    <t>/Users/David/Documents/projects/mastergui/data/hcp_comm_det_damien/cub-sub-NDARINV02EBX0JJ_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
-  </si>
-  <si>
-    <t>/Users/David/Documents/projects/mastergui/data/hcp_comm_det_damien/cub-sub-NDARINV0U23M45G_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
-  </si>
-  <si>
-    <t>/Users/David/Documents/projects/mastergui/data/hcp_comm_det_damien/cub-sub-NDARINV1K3LDK3L_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
-  </si>
-  <si>
-    <t>/Users/David/Documents/projects/mastergui/data/hcp_comm_det_damien/cub-sub-NDARINV1V7XPJKR_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
-  </si>
-  <si>
-    <t>/Users/David/Documents/projects/mastergui/data/hcp_comm_det_damien/cub-sub-NDARINV7Y7JEGPW_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+    <t>data/hcp_comm_det_damien/cub-sub-NDARINV02EBX0JJ_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+  </si>
+  <si>
+    <t>data/hcp_comm_det_damien/cub-sub-NDARINV0U23M45G_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+  </si>
+  <si>
+    <t>data/hcp_comm_det_damien/cub-sub-NDARINV1K3LDK3L_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+  </si>
+  <si>
+    <t>data/hcp_comm_det_damien/cub-sub-NDARINV1V7XPJKR_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+  </si>
+  <si>
+    <t>data/hcp_comm_det_damien/cub-sub-NDARINV7Y7JEGPW_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
add support for multiple voxel columns
</commit_message>
<xml_diff>
--- a/tests/input_csv_file_test_case_Evan_simple.xlsx
+++ b/tests/input_csv_file_test_case_Evan_simple.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>ID_SUBJ</t>
   </si>
@@ -46,9 +46,6 @@
     <t>PATH_HCP</t>
   </si>
   <si>
-    <t>.</t>
-  </si>
-  <si>
     <t>data/hcp_comm_det_damien/cub-sub-NDARINV02EBX0JJ_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
   </si>
   <si>
@@ -62,6 +59,9 @@
   </si>
   <si>
     <t>data/hcp_comm_det_damien/cub-sub-NDARINV7Y7JEGPW_FNL_preproc_v2_Atlas_SMOOTHED_1.7.dtseries.nii_10_minutes_of_data_at_FD_0.2.dconn.nii_to_Merged_HCP_best80_dtseries.conc_AVG.dconn.dscalar.nii</t>
+  </si>
+  <si>
+    <t>PATH_HCP2</t>
   </si>
 </sst>
 </file>
@@ -110,17 +110,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -468,7 +472,7 @@
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,8 +497,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>110461</v>
       </c>
@@ -517,10 +524,13 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>110461</v>
       </c>
@@ -528,7 +538,7 @@
         <v>20120211</v>
       </c>
       <c r="C3">
-        <v>-888</v>
+        <v>8.071185582</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -543,10 +553,13 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>102861</v>
       </c>
@@ -554,13 +567,13 @@
         <v>20110315</v>
       </c>
       <c r="C4">
-        <v>-888</v>
+        <v>8.5054758140000004</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="E4">
+        <v>120</v>
       </c>
       <c r="F4">
         <v>0.114010396</v>
@@ -569,10 +582,13 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>102861</v>
       </c>
@@ -582,6 +598,9 @@
       <c r="C5">
         <v>8.5054758140000004</v>
       </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
       <c r="E5">
         <v>120</v>
       </c>
@@ -592,10 +611,13 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>104882</v>
       </c>
@@ -611,14 +633,20 @@
       <c r="E6">
         <v>127</v>
       </c>
+      <c r="F6">
+        <v>0.112099692</v>
+      </c>
       <c r="G6">
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>104882</v>
       </c>
@@ -634,14 +662,20 @@
       <c r="E7">
         <v>127</v>
       </c>
+      <c r="F7">
+        <v>0.14724352399999999</v>
+      </c>
       <c r="G7">
         <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>108451</v>
       </c>
@@ -654,17 +688,23 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
+      <c r="E8">
+        <v>106</v>
+      </c>
+      <c r="F8">
+        <v>9.8611654000000007E-2</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>108451</v>
       </c>
@@ -680,14 +720,20 @@
       <c r="E9">
         <v>106</v>
       </c>
+      <c r="F9">
+        <v>0.12264222599999999</v>
+      </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>110741</v>
       </c>
@@ -710,10 +756,13 @@
         <v>5</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>11</v>
+      </c>
+      <c r="I10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>110741</v>
       </c>
@@ -736,7 +785,10 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parellelizing the csv generation step and adding a robust test of its success
</commit_message>
<xml_diff>
--- a/tests/input_csv_file_test_case_Evan_simple.xlsx
+++ b/tests/input_csv_file_test_case_Evan_simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="2200" windowWidth="27640" windowHeight="13860"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="27640" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="test_case_Evan" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -110,8 +111,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -120,11 +133,23 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,7 +482,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -527,7 +552,7 @@
         <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -553,10 +578,10 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9">

</xml_diff>